<commit_message>
updated with leave-one-out data for DL stuff
</commit_message>
<xml_diff>
--- a/Analysis/CV Data Analysis.xlsx
+++ b/Analysis/CV Data Analysis.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6d033e4df2e0e342/Documents/JHU/2020 Fall/Computer_Vision-jpsoong/Final_Project/finger_detection/Analysis/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="114_{FF29CC47-0B01-488E-8175-EBA755E92D65}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="570" yWindow="3450" windowWidth="21915" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Test" sheetId="1" r:id="rId1"/>
     <sheet name="Validation" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -86,8 +92,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -150,6 +156,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -196,7 +210,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -228,9 +242,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -262,6 +294,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -437,14 +487,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -467,7 +517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -493,7 +543,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -519,7 +569,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -545,7 +595,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -571,7 +621,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -597,7 +647,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -623,7 +673,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -649,7 +699,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -675,7 +725,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -701,7 +751,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -727,7 +777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -753,7 +803,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -779,7 +829,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -805,7 +855,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -831,7 +881,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -857,7 +907,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -883,7 +933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -909,7 +959,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -935,7 +985,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -961,7 +1011,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -987,7 +1037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1013,7 +1063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1039,7 +1089,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1065,7 +1115,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1091,7 +1141,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1117,7 +1167,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1143,7 +1193,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1169,7 +1219,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1195,7 +1245,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1221,7 +1271,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1247,7 +1297,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1273,7 +1323,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1299,7 +1349,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1325,7 +1375,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1351,7 +1401,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1377,7 +1427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1403,7 +1453,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1429,7 +1479,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1455,7 +1505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1481,7 +1531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1507,7 +1557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1533,7 +1583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1559,7 +1609,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1585,7 +1635,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1611,7 +1661,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1637,7 +1687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1663,7 +1713,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1689,7 +1739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1715,7 +1765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1741,7 +1791,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1767,7 +1817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1793,7 +1843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1819,7 +1869,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1845,7 +1895,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1871,7 +1921,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1897,7 +1947,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1923,7 +1973,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1949,7 +1999,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1975,7 +2025,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2001,7 +2051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2027,7 +2077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2053,7 +2103,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2079,7 +2129,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2105,7 +2155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2131,7 +2181,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2157,7 +2207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2183,7 +2233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2209,7 +2259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2235,7 +2285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2261,7 +2311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2287,7 +2337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2313,7 +2363,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2339,7 +2389,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2365,7 +2415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2391,7 +2441,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2417,7 +2467,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2443,7 +2493,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2469,7 +2519,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2495,7 +2545,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2521,7 +2571,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2547,7 +2597,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2573,7 +2623,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2599,7 +2649,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2625,7 +2675,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2651,7 +2701,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2677,7 +2727,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2703,7 +2753,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2729,7 +2779,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2755,7 +2805,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2781,7 +2831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2807,7 +2857,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2833,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2859,7 +2909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2885,7 +2935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2911,7 +2961,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -2937,7 +2987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -2963,7 +3013,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -2989,7 +3039,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3015,7 +3065,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3041,7 +3091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3067,7 +3117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3093,7 +3143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3119,7 +3169,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3145,7 +3195,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3171,7 +3221,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3197,7 +3247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3223,7 +3273,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3249,7 +3299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3275,7 +3325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3301,7 +3351,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3327,7 +3377,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3353,7 +3403,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -3379,7 +3429,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3405,7 +3455,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3431,7 +3481,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3457,7 +3507,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -3483,7 +3533,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -3509,7 +3559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -3535,7 +3585,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -3561,7 +3611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3587,7 +3637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -3613,7 +3663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -3639,7 +3689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -3665,7 +3715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -3691,7 +3741,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -3717,7 +3767,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -3743,7 +3793,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -3769,7 +3819,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -3795,7 +3845,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -3821,7 +3871,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -3847,7 +3897,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -3873,7 +3923,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -3899,7 +3949,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -3925,7 +3975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -3951,7 +4001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -3977,7 +4027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -4003,7 +4053,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -4029,7 +4079,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -4055,7 +4105,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -4081,7 +4131,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="141" spans="1:8">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -4107,7 +4157,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="142" spans="1:8">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -4133,7 +4183,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="143" spans="1:8">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -4159,7 +4209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="144" spans="1:8">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -4185,7 +4235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="145" spans="1:8">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -4211,7 +4261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="146" spans="1:8">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -4237,7 +4287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="147" spans="1:8">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -4263,7 +4313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:8">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -4289,7 +4339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:8">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -4315,7 +4365,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:8">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -4341,7 +4391,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="151" spans="1:8">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -4367,7 +4417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="152" spans="1:8">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -4393,7 +4443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="153" spans="1:8">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -4419,7 +4469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="154" spans="1:8">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -4445,7 +4495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="155" spans="1:8">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -4471,7 +4521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="156" spans="1:8">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -4497,7 +4547,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="157" spans="1:8">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -4523,7 +4573,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:8">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -4549,7 +4599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="159" spans="1:8">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -4575,7 +4625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="160" spans="1:8">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -4601,7 +4651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:8">
+    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -4627,7 +4677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="162" spans="1:8">
+    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -4653,7 +4703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:8">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -4679,7 +4729,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:8">
+    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -4705,7 +4755,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:8">
+    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -4731,7 +4781,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:8">
+    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -4757,7 +4807,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="167" spans="1:8">
+    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -4783,7 +4833,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="168" spans="1:8">
+    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -4809,7 +4859,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="169" spans="1:8">
+    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -4835,7 +4885,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="170" spans="1:8">
+    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -4861,7 +4911,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="171" spans="1:8">
+    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -4887,7 +4937,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="172" spans="1:8">
+    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -4913,7 +4963,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="173" spans="1:8">
+    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -4939,7 +4989,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="174" spans="1:8">
+    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -4965,7 +5015,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="175" spans="1:8">
+    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -4991,7 +5041,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="176" spans="1:8">
+    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -5017,7 +5067,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="177" spans="1:8">
+    <row r="177" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -5043,7 +5093,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="178" spans="1:8">
+    <row r="178" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -5069,7 +5119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="179" spans="1:8">
+    <row r="179" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -5095,7 +5145,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="180" spans="1:8">
+    <row r="180" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -5121,7 +5171,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="1:8">
+    <row r="181" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -5147,7 +5197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:8">
+    <row r="182" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -5173,7 +5223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="183" spans="1:8">
+    <row r="183" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -5199,7 +5249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:8">
+    <row r="184" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -5225,7 +5275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="185" spans="1:8">
+    <row r="185" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -5251,7 +5301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="186" spans="1:8">
+    <row r="186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -5277,7 +5327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="1:8">
+    <row r="187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -5303,7 +5353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="188" spans="1:8">
+    <row r="188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -5329,7 +5379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="189" spans="1:8">
+    <row r="189" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -5355,7 +5405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="190" spans="1:8">
+    <row r="190" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -5381,7 +5431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="191" spans="1:8">
+    <row r="191" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -5407,7 +5457,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="192" spans="1:8">
+    <row r="192" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -5433,7 +5483,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="193" spans="1:8">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -5459,7 +5509,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="194" spans="1:8">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -5485,7 +5535,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="195" spans="1:8">
+    <row r="195" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -5511,7 +5561,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="196" spans="1:8">
+    <row r="196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -5537,7 +5587,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="197" spans="1:8">
+    <row r="197" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -5563,7 +5613,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="198" spans="1:8">
+    <row r="198" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -5589,7 +5639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="199" spans="1:8">
+    <row r="199" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -5615,7 +5665,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="200" spans="1:8">
+    <row r="200" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -5641,7 +5691,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="201" spans="1:8">
+    <row r="201" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -5667,7 +5717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:8">
+    <row r="202" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -5693,7 +5743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:8">
+    <row r="203" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -5719,7 +5769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:8">
+    <row r="204" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -5745,7 +5795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:8">
+    <row r="205" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -5771,7 +5821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="206" spans="1:8">
+    <row r="206" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -5797,7 +5847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="207" spans="1:8">
+    <row r="207" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -5823,7 +5873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="208" spans="1:8">
+    <row r="208" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -5849,7 +5899,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="209" spans="1:8">
+    <row r="209" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -5875,7 +5925,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="210" spans="1:8">
+    <row r="210" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -5901,7 +5951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="211" spans="1:8">
+    <row r="211" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -5927,7 +5977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="212" spans="1:8">
+    <row r="212" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -5953,7 +6003,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="213" spans="1:8">
+    <row r="213" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -5979,7 +6029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="214" spans="1:8">
+    <row r="214" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -6005,7 +6055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="215" spans="1:8">
+    <row r="215" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -6031,7 +6081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="216" spans="1:8">
+    <row r="216" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -6057,7 +6107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="217" spans="1:8">
+    <row r="217" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -6083,7 +6133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="218" spans="1:8">
+    <row r="218" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -6109,7 +6159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="219" spans="1:8">
+    <row r="219" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -6141,14 +6191,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H140"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6171,7 +6221,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -6197,7 +6247,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -6223,7 +6273,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -6249,7 +6299,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -6275,7 +6325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -6301,7 +6351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -6327,7 +6377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -6353,7 +6403,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -6379,7 +6429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -6405,7 +6455,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -6431,7 +6481,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -6457,7 +6507,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -6483,7 +6533,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -6509,7 +6559,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -6535,7 +6585,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -6561,7 +6611,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -6587,7 +6637,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -6613,7 +6663,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -6639,7 +6689,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -6665,7 +6715,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -6691,7 +6741,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -6717,7 +6767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -6743,7 +6793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -6769,7 +6819,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -6795,7 +6845,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -6821,7 +6871,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -6847,7 +6897,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -6873,7 +6923,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -6899,7 +6949,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -6925,7 +6975,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -6951,7 +7001,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -6977,7 +7027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -7003,7 +7053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -7029,7 +7079,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -7055,7 +7105,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -7081,7 +7131,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -7107,7 +7157,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -7133,7 +7183,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -7159,7 +7209,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -7185,7 +7235,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:8">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -7211,7 +7261,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:8">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -7237,7 +7287,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:8">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -7263,7 +7313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:8">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -7289,7 +7339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:8">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -7315,7 +7365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:8">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -7341,7 +7391,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -7367,7 +7417,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -7393,7 +7443,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -7419,7 +7469,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:8">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -7445,7 +7495,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="51" spans="1:8">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -7471,7 +7521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="52" spans="1:8">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -7497,7 +7547,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:8">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -7523,7 +7573,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -7549,7 +7599,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="55" spans="1:8">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -7575,7 +7625,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:8">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -7601,7 +7651,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="57" spans="1:8">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -7627,7 +7677,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:8">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -7653,7 +7703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:8">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -7679,7 +7729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:8">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -7705,7 +7755,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:8">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -7731,7 +7781,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:8">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -7757,7 +7807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:8">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -7783,7 +7833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -7809,7 +7859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -7835,7 +7885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -7861,7 +7911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -7887,7 +7937,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:8">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -7913,7 +7963,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="69" spans="1:8">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -7939,7 +7989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:8">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -7965,7 +8015,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -7991,7 +8041,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="72" spans="1:8">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -8017,7 +8067,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="1:8">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -8043,7 +8093,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:8">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -8069,7 +8119,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:8">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -8095,7 +8145,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:8">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -8121,7 +8171,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:8">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -8147,7 +8197,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -8173,7 +8223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -8199,7 +8249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -8225,7 +8275,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -8251,7 +8301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -8277,7 +8327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -8303,7 +8353,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -8329,7 +8379,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:8">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -8355,7 +8405,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="86" spans="1:8">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -8381,7 +8431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:8">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -8407,7 +8457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -8433,7 +8483,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="89" spans="1:8">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -8459,7 +8509,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="90" spans="1:8">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -8485,7 +8535,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="91" spans="1:8">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -8511,7 +8561,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:8">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -8537,7 +8587,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -8563,7 +8613,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -8589,7 +8639,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="95" spans="1:8">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -8615,7 +8665,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:8">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -8641,7 +8691,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:8">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -8667,7 +8717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:8">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -8693,7 +8743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:8">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -8719,7 +8769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:8">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -8745,7 +8795,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:8">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -8771,7 +8821,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="102" spans="1:8">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -8797,7 +8847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="103" spans="1:8">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -8823,7 +8873,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="104" spans="1:8">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -8849,7 +8899,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:8">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -8875,7 +8925,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:8">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -8901,7 +8951,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="107" spans="1:8">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -8927,7 +8977,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="108" spans="1:8">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -8953,7 +9003,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -8979,7 +9029,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="110" spans="1:8">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -9005,7 +9055,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="111" spans="1:8">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -9031,7 +9081,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="112" spans="1:8">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -9057,7 +9107,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -9083,7 +9133,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -9109,7 +9159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -9135,7 +9185,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -9161,7 +9211,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -9187,7 +9237,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -9213,7 +9263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:8">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -9239,7 +9289,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="120" spans="1:8">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -9265,7 +9315,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="1:8">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -9291,7 +9341,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:8">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -9317,7 +9367,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="123" spans="1:8">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -9343,7 +9393,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="124" spans="1:8">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -9369,7 +9419,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="125" spans="1:8">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -9395,7 +9445,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:8">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -9421,7 +9471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:8">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -9447,7 +9497,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="128" spans="1:8">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -9473,7 +9523,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="129" spans="1:8">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -9499,7 +9549,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="130" spans="1:8">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -9525,7 +9575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="131" spans="1:8">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -9551,7 +9601,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="132" spans="1:8">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -9577,7 +9627,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -9603,7 +9653,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="134" spans="1:8">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -9629,7 +9679,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="135" spans="1:8">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -9655,7 +9705,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:8">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -9681,7 +9731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:8">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -9707,7 +9757,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="138" spans="1:8">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -9733,7 +9783,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="139" spans="1:8">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -9759,7 +9809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" spans="1:8">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" s="1">
         <v>138</v>
       </c>

</xml_diff>